<commit_message>
headless mode & purge done
</commit_message>
<xml_diff>
--- a/donnees_sortie.xlsx
+++ b/donnees_sortie.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>FRP société</t>
   </si>
@@ -34,13 +34,7 @@
     <t>Fait</t>
   </si>
   <si>
-    <t>AAA977</t>
-  </si>
-  <si>
-    <t>AAA978</t>
-  </si>
-  <si>
-    <t>AAA979</t>
+    <t>AAA990</t>
   </si>
   <si>
     <t>X</t>
@@ -418,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -470,53 +464,7 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>617382</v>
-      </c>
-      <c r="C3">
-        <v>203268</v>
-      </c>
-      <c r="D3">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3">
-        <v>44915</v>
-      </c>
-      <c r="F3" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>617382</v>
-      </c>
-      <c r="C4">
-        <v>203268</v>
-      </c>
-      <c r="D4">
-        <v>87</v>
-      </c>
-      <c r="E4" s="3">
-        <v>44916</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>